<commit_message>
Ajout d'espèces et modification des régimes dans le script
</commit_message>
<xml_diff>
--- a/Fichiers modifiables/ListeEspèces.xlsx
+++ b/Fichiers modifiables/ListeEspèces.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Trimestre 6\MA 08 - Serveur BD\Ma-08_Zoo\Fichiers modifiables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Trimestre 6\MA 08 - Serveur BD\Ma-08_Zoo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="122">
   <si>
     <t>name</t>
   </si>
@@ -35,12 +35,12 @@
     <t>status_id</t>
   </si>
   <si>
-    <t>LC</t>
-  </si>
-  <si>
     <t>Habitat</t>
   </si>
   <si>
+    <t>Forêts</t>
+  </si>
+  <si>
     <t>Alligator du Mississippi</t>
   </si>
   <si>
@@ -62,9 +62,6 @@
     <t>Buceros rhinoceros sylvestris</t>
   </si>
   <si>
-    <t>VU</t>
-  </si>
-  <si>
     <t>omnivore</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>Pteropus rodricensis</t>
   </si>
   <si>
-    <t>EN</t>
-  </si>
-  <si>
     <t>frugivore</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Gorille des plaines de l'Ouest</t>
   </si>
   <si>
-    <t>CR</t>
-  </si>
-  <si>
     <t>Gorilla gorilla gorilla</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>Gypaète barbu</t>
   </si>
   <si>
-    <t>NT</t>
-  </si>
-  <si>
     <t>Gypaetus barbatus</t>
   </si>
   <si>
@@ -242,13 +230,166 @@
     <t>-</t>
   </si>
   <si>
-    <t>NE</t>
-  </si>
-  <si>
     <t>forêt</t>
   </si>
   <si>
     <t>Informations tirées de : https://www.zoobeauval.com/zooparc/liste-des-animaux</t>
+  </si>
+  <si>
+    <t>Tapir terrestre</t>
+  </si>
+  <si>
+    <t>Tapirus terrestris</t>
+  </si>
+  <si>
+    <t>Suricata suricatta</t>
+  </si>
+  <si>
+    <t>Suricate</t>
+  </si>
+  <si>
+    <t>Savanes, Milieux arides</t>
+  </si>
+  <si>
+    <t>Rhinocéros indien</t>
+  </si>
+  <si>
+    <t>Rhinoceros unicornis</t>
+  </si>
+  <si>
+    <t>Prairies, Milieux humides, Forêts tropicales</t>
+  </si>
+  <si>
+    <t>Rhinocéros blanc du Sud</t>
+  </si>
+  <si>
+    <t>Ceratotherium simum simum</t>
+  </si>
+  <si>
+    <t>Raton laveur</t>
+  </si>
+  <si>
+    <t>Procyon lotor</t>
+  </si>
+  <si>
+    <t>Tous types d'habitats</t>
+  </si>
+  <si>
+    <t>Paresseux à deux doigts</t>
+  </si>
+  <si>
+    <t>Choloepus didactylus</t>
+  </si>
+  <si>
+    <t>Panthère des neiges</t>
+  </si>
+  <si>
+    <t>Panthera uncia</t>
+  </si>
+  <si>
+    <t>Panda géant</t>
+  </si>
+  <si>
+    <t>Ailuropoda melanoleuca</t>
+  </si>
+  <si>
+    <t>Forêts de montagne</t>
+  </si>
+  <si>
+    <t>Panda roux</t>
+  </si>
+  <si>
+    <t>Ailurus fulgens</t>
+  </si>
+  <si>
+    <t>Otaries de Californie</t>
+  </si>
+  <si>
+    <t>Zalophus californianus</t>
+  </si>
+  <si>
+    <t>Eaux salées, Côte rocheuse</t>
+  </si>
+  <si>
+    <t>Orang-outan de Bornéo</t>
+  </si>
+  <si>
+    <t>Pongo pygmaeus</t>
+  </si>
+  <si>
+    <t>Okapi</t>
+  </si>
+  <si>
+    <t>Okapia johnstoni</t>
+  </si>
+  <si>
+    <t>Folivore</t>
+  </si>
+  <si>
+    <t>Microglosse</t>
+  </si>
+  <si>
+    <t>Probosciger aterrimus</t>
+  </si>
+  <si>
+    <t>Frugivore, Granivore</t>
+  </si>
+  <si>
+    <t>Savanes arborées, Forêts tropicales</t>
+  </si>
+  <si>
+    <t>Manchot de Humboldt</t>
+  </si>
+  <si>
+    <t>Spheniscus humboldti</t>
+  </si>
+  <si>
+    <t>Piscivore</t>
+  </si>
+  <si>
+    <t>Côte rocheuse</t>
+  </si>
+  <si>
+    <t>Maki catta</t>
+  </si>
+  <si>
+    <t>Lemur catta</t>
+  </si>
+  <si>
+    <t>Magot</t>
+  </si>
+  <si>
+    <t>Macaca sylvanus</t>
+  </si>
+  <si>
+    <t>Omnivore, Frugivore</t>
+  </si>
+  <si>
+    <t>Montagnes, Forêts</t>
+  </si>
+  <si>
+    <t>Loutre géante</t>
+  </si>
+  <si>
+    <t>Pteronura brasiliensis</t>
+  </si>
+  <si>
+    <t>Loutre naine d'Asie</t>
+  </si>
+  <si>
+    <t>Aonyx cinereus</t>
+  </si>
+  <si>
+    <t>Eaux douces</t>
+  </si>
+  <si>
+    <t>Loup arctique</t>
+  </si>
+  <si>
+    <t>Canis lupus arctos</t>
+  </si>
+  <si>
+    <t>Toundra Arctique</t>
   </si>
 </sst>
 </file>
@@ -284,8 +425,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,87 +443,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>143007</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>181204</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3771900" y="257175"/>
-          <a:ext cx="943107" cy="1638529"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>28840</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>66941</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4991100" y="257175"/>
-          <a:ext cx="1895740" cy="1905266"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +733,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -685,8 +746,8 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
+      <c r="D2" s="1">
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -700,327 +761,649 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
+      <c r="D4" s="1">
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
+      <c r="D8" s="1">
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
+      <c r="D12" s="1">
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
         <v>52</v>
-      </c>
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
+        <v>22</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
+      <c r="D19" s="1">
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="s">
-        <v>45</v>
+      <c r="D20" s="1">
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="1">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
         <v>72</v>
       </c>
-      <c r="E21" t="s">
-        <v>73</v>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="1">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
+        <v>99</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D34" s="1">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="1">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="1">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="1">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+      <c r="C38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="1">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de nouvelles espèces
</commit_message>
<xml_diff>
--- a/Fichiers modifiables/ListeEspèces.xlsx
+++ b/Fichiers modifiables/ListeEspèces.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Trimestre 6\MA 08 - Serveur BD\Ma-08_Zoo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Trimestre 6\MA 08 - Serveur BD\Ma-08_Zoo\Fichiers modifiables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -150,6 +150,33 @@
   </si>
   <si>
     <t>Pika de pallas</t>
+  </si>
+  <si>
+    <t>Python royal</t>
+  </si>
+  <si>
+    <t>Tortue léopard</t>
+  </si>
+  <si>
+    <t>Scorpion</t>
+  </si>
+  <si>
+    <t>Mante religieuse</t>
+  </si>
+  <si>
+    <t>Dragon barbu de l'Est</t>
+  </si>
+  <si>
+    <t>Caméléon panthère</t>
+  </si>
+  <si>
+    <t>Sonneur oritental</t>
+  </si>
+  <si>
+    <t>Tarentule vraie</t>
+  </si>
+  <si>
+    <t>Rainette arboricole</t>
   </si>
 </sst>
 </file>
@@ -479,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,6 +959,116 @@
       </c>
       <c r="D40" s="2"/>
     </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41">
+        <v>8</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>8</v>
+      </c>
+      <c r="C45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>